<commit_message>
Debug envoie d'info + estimation
</commit_message>
<xml_diff>
--- a/Synopsys/estimation.xlsx
+++ b/Synopsys/estimation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Se refamiliariser avec android et java était un peu plus hardu que prévu.</t>
+  </si>
+  <si>
+    <t>Debugger l'envoie de donner + recherche de addContentView</t>
   </si>
 </sst>
 </file>
@@ -1883,7 +1886,7 @@
   <dimension ref="A6:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1984,9 +1987,15 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="18">
+        <v>43185</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
@@ -2085,7 +2094,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Debugger l'alertdialog + estimation
</commit_message>
<xml_diff>
--- a/Synopsys/estimation.xlsx
+++ b/Synopsys/estimation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Debugger l'envoie de donner + recherche de addContentView</t>
+  </si>
+  <si>
+    <t>Debugger l'alertdialog</t>
   </si>
 </sst>
 </file>
@@ -1885,8 +1888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1998,9 +2001,15 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
+      <c r="A19" s="18">
+        <v>43186</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
@@ -2094,7 +2103,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fin debug AlertDialog + debug PendingIntent
</commit_message>
<xml_diff>
--- a/Synopsys/estimation.xlsx
+++ b/Synopsys/estimation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Debugger l'alertdialog</t>
+  </si>
+  <si>
+    <t>Fin debug alertDialog + debug pendingIntent</t>
   </si>
 </sst>
 </file>
@@ -1888,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2012,9 +2015,15 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="18">
+        <v>43187</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
@@ -2103,7 +2112,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Mise à jour de extimation
</commit_message>
<xml_diff>
--- a/Synopsys/estimation.xlsx
+++ b/Synopsys/estimation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Semaine 15</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Le projet doit être décomposé en plusieurs sections indépendantes qui doivent être priorisées et estimées</t>
   </si>
   <si>
@@ -189,6 +186,12 @@
   </si>
   <si>
     <t>Debug AsyncTask</t>
+  </si>
+  <si>
+    <t>Debug service + fin debug asynctask</t>
+  </si>
+  <si>
+    <t>fin debug service + aide francois-oli</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1657,7 @@
   <sheetData>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1669,12 +1672,12 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1699,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3">
         <v>15</v>
@@ -1710,7 +1713,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3">
         <v>18</v>
@@ -1721,7 +1724,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="3">
         <v>15</v>
@@ -1732,7 +1735,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3">
         <v>15</v>
@@ -1743,7 +1746,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3">
         <v>15</v>
@@ -1786,7 +1789,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="3">
         <v>10</v>
@@ -1797,7 +1800,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="3">
         <v>10</v>
@@ -1808,7 +1811,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="3">
         <v>5</v>
@@ -1819,7 +1822,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3">
         <v>5</v>
@@ -1830,7 +1833,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="3">
         <v>5</v>
@@ -1841,7 +1844,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="3">
         <v>3</v>
@@ -1852,7 +1855,7 @@
         <v>7</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="3">
         <v>10</v>
@@ -1863,7 +1866,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="3">
         <v>20</v>
@@ -1962,7 +1965,7 @@
         <v>43178</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="15">
         <v>3</v>
@@ -1973,7 +1976,7 @@
         <v>43179</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="15">
         <v>5</v>
@@ -1984,7 +1987,7 @@
         <v>43180</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="15">
         <v>6</v>
@@ -1995,7 +1998,7 @@
         <v>43181</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="15">
         <v>3</v>
@@ -2006,7 +2009,7 @@
         <v>43185</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="15">
         <v>3</v>
@@ -2017,7 +2020,7 @@
         <v>43186</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="15">
         <v>2</v>
@@ -2028,7 +2031,7 @@
         <v>43187</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="15">
         <v>3</v>
@@ -2126,13 +2129,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="4">
         <v>7</v>
@@ -2143,10 +2146,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -2179,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2241,7 +2244,7 @@
         <v>43194</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="15">
         <v>3</v>
@@ -2252,7 +2255,7 @@
         <v>43195</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="15">
         <v>5</v>
@@ -2263,23 +2266,33 @@
         <v>43199</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="18">
+        <v>43202</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="18">
+        <v>43206</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
@@ -2378,18 +2391,18 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2398,7 +2411,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="21"/>
     </row>
@@ -2616,13 +2629,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2631,7 +2644,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="21"/>
     </row>
@@ -2702,7 +2715,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2849,13 +2862,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2864,7 +2877,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="21"/>
     </row>

</xml_diff>

<commit_message>
début de l'Implémentation de SQLite
</commit_message>
<xml_diff>
--- a/Synopsys/estimation.xlsx
+++ b/Synopsys/estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>fin debug service + aide francois-oli</t>
+  </si>
+  <si>
+    <t>Aucun commentaire, tout c'est bien déroulé.</t>
+  </si>
+  <si>
+    <t>Debut de l'implémentation de SQLite dans l'app</t>
   </si>
 </sst>
 </file>
@@ -1644,7 +1650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C36"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -2182,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView view="pageLayout" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2247,7 +2253,7 @@
         <v>53</v>
       </c>
       <c r="C14" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -2291,7 +2297,7 @@
         <v>57</v>
       </c>
       <c r="C18" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2391,7 +2397,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2404,7 +2410,9 @@
       <c r="A40" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="7"/>
@@ -2413,7 +2421,9 @@
       <c r="A42" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="21" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B43" s="22"/>
@@ -2445,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2503,9 +2513,15 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>43213</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
@@ -2624,7 +2640,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Implementation de la bd plus debug
</commit_message>
<xml_diff>
--- a/Synopsys/estimation.xlsx
+++ b/Synopsys/estimation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Debut de l'implémentation de SQLite dans l'app</t>
+  </si>
+  <si>
+    <t>Suite implémentation de la BD dans l'app</t>
   </si>
 </sst>
 </file>
@@ -2455,8 +2458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2520,18 +2523,30 @@
         <v>59</v>
       </c>
       <c r="C14" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="18">
+        <v>43214</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="18">
+        <v>43215</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
@@ -2640,7 +2655,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Debug btnLogin + debug SQLite + debug + debug gameplayActivity
</commit_message>
<xml_diff>
--- a/Synopsys/estimation.xlsx
+++ b/Synopsys/estimation.xlsx
@@ -2459,7 +2459,7 @@
   <dimension ref="A6:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2545,7 +2545,7 @@
         <v>60</v>
       </c>
       <c r="C16" s="15">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2655,7 +2655,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Suite implémentation dans l'app
</commit_message>
<xml_diff>
--- a/Synopsys/estimation.xlsx
+++ b/Synopsys/estimation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -1912,7 +1912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -2191,7 +2191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
@@ -2458,8 +2458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2549,14 +2549,26 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="18">
+        <v>43220</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="18">
+        <v>43221</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
@@ -2655,7 +2667,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>